<commit_message>
JS08 - Refactor: fitur import data supplier
</commit_message>
<xml_diff>
--- a/public/template_supplier.xlsx
+++ b/public/template_supplier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0277E80E-8FC7-429E-94AA-9ED52650FC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AE910E-C80D-4227-8CE9-1D4C197D7279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="760" windowWidth="11330" windowHeight="8080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>supplier_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>supplier_kode</t>
   </si>
@@ -407,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,7 +418,7 @@
     <col min="4" max="4" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,50 +428,38 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>